<commit_message>
ตรวจ Burndown & Velocity Sprint 7
</commit_message>
<xml_diff>
--- a/ตรวจงาน/รายการตรวจสอบเอกสารอื่น ๆ.xlsx
+++ b/ตรวจงาน/รายการตรวจสอบเอกสารอื่น ๆ.xlsx
@@ -5,27 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nice-\Desktop\Porn\team4\ตรวจงาน\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\team4\ตรวจงาน\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE961685-57C3-499E-B216-DAFD8B513034}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8743BE70-F858-4D20-83CF-06191B77747F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="3735" windowWidth="21600" windowHeight="11835" xr2:uid="{C108298C-C5B1-4B19-85F2-2856099ECD84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C108298C-C5B1-4B19-85F2-2856099ECD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>คำผิด</t>
   </si>
@@ -140,16 +149,22 @@
   <si>
     <t>1.7.1</t>
   </si>
+  <si>
+    <t>Burndown Velocity Sprint 1-7</t>
+  </si>
+  <si>
+    <t>1.8.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -169,7 +184,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -236,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -274,13 +289,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -292,9 +304,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -310,7 +328,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -608,116 +626,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E552DF3-66E3-4350-8BDE-D3162A98C3B8}">
   <dimension ref="B2:X166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.69921875" style="1"/>
+    <col min="2" max="2" width="29.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" style="1"/>
+    <col min="4" max="4" width="10.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="50.45" customHeight="1">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:24" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:24" ht="51.75" customHeight="1">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-    </row>
-    <row r="4" spans="2:24" ht="30" customHeight="1">
+    <row r="3" spans="2:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+    </row>
+    <row r="4" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -767,7 +785,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:24" ht="30" customHeight="1">
+    <row r="5" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -802,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:24" ht="30" customHeight="1">
+    <row r="6" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
@@ -837,7 +855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:24" ht="30" customHeight="1">
+    <row r="7" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
@@ -872,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="30" customHeight="1">
+    <row r="8" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
@@ -916,7 +934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:24" ht="30" customHeight="1">
+    <row r="9" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
@@ -957,7 +975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:24" ht="30" customHeight="1">
+    <row r="10" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -994,11 +1012,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:24" ht="30" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+    <row r="11" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4">
+        <v>44425</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1017,9 +1043,11 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-    </row>
-    <row r="12" spans="2:24" ht="30" customHeight="1">
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B12" s="6"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1044,7 +1072,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="2:24" ht="30" customHeight="1">
+    <row r="13" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B13" s="6"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1069,7 +1097,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="2:24" ht="30" customHeight="1">
+    <row r="14" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B14" s="6"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1094,7 +1122,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="2:24" ht="30" customHeight="1">
+    <row r="15" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B15" s="6"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1119,7 +1147,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="2:24" ht="30" customHeight="1">
+    <row r="16" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B16" s="6"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1144,7 +1172,7 @@
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="2:24" ht="30" customHeight="1">
+    <row r="17" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B17" s="6"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1169,7 +1197,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="2:24" ht="30" customHeight="1">
+    <row r="18" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1194,7 +1222,7 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="2:24" ht="30" customHeight="1">
+    <row r="19" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1219,7 +1247,7 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="2:24" ht="30" customHeight="1">
+    <row r="20" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B20" s="6"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1244,7 +1272,7 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="2:24" ht="30" customHeight="1">
+    <row r="21" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B21" s="6"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1269,7 +1297,7 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="2:24" ht="30" customHeight="1">
+    <row r="22" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B22" s="6"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1294,7 +1322,7 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="2:24" ht="30" customHeight="1">
+    <row r="23" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B23" s="6"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1319,7 +1347,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="2:24" ht="30" customHeight="1">
+    <row r="24" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1344,7 +1372,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="2:24" ht="30" customHeight="1">
+    <row r="25" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B25" s="6"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1369,7 +1397,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="2:24" ht="30" customHeight="1">
+    <row r="26" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1394,7 +1422,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="2:24" ht="30" customHeight="1">
+    <row r="27" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B27" s="6"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1419,7 +1447,7 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="2:24" ht="30" customHeight="1">
+    <row r="28" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B28" s="6"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1444,7 +1472,7 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="2:24" ht="30" customHeight="1">
+    <row r="29" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B29" s="6"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1469,7 +1497,7 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="2:24" ht="30" customHeight="1">
+    <row r="30" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B30" s="6"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1494,7 +1522,7 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" spans="2:24" ht="30" customHeight="1">
+    <row r="31" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B31" s="6"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1519,7 +1547,7 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" spans="2:24" ht="30" customHeight="1">
+    <row r="32" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B32" s="6"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1544,7 +1572,7 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" spans="2:24" ht="30" customHeight="1">
+    <row r="33" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B33" s="6"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1569,7 +1597,7 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
     </row>
-    <row r="34" spans="2:24" ht="30" customHeight="1">
+    <row r="34" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B34" s="6"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1594,7 +1622,7 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" spans="2:24" ht="30" customHeight="1">
+    <row r="35" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B35" s="6"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1619,7 +1647,7 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
     </row>
-    <row r="36" spans="2:24" ht="30" customHeight="1">
+    <row r="36" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B36" s="6"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1644,7 +1672,7 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="2:24" ht="30" customHeight="1">
+    <row r="37" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B37" s="6"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1669,7 +1697,7 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="2:24" ht="30" customHeight="1">
+    <row r="38" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B38" s="6"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1694,7 +1722,7 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" spans="2:24" ht="30" customHeight="1">
+    <row r="39" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B39" s="6"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1719,7 +1747,7 @@
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
     </row>
-    <row r="40" spans="2:24" ht="30" customHeight="1">
+    <row r="40" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B40" s="6"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1744,7 +1772,7 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" spans="2:24" ht="30" customHeight="1">
+    <row r="41" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B41" s="6"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1769,7 +1797,7 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" spans="2:24" ht="30" customHeight="1">
+    <row r="42" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B42" s="6"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1794,7 +1822,7 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="2:24" ht="30" customHeight="1">
+    <row r="43" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B43" s="6"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1819,7 +1847,7 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
     </row>
-    <row r="44" spans="2:24" ht="30" customHeight="1">
+    <row r="44" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B44" s="6"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1844,7 +1872,7 @@
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
     </row>
-    <row r="45" spans="2:24" ht="30" customHeight="1">
+    <row r="45" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B45" s="6"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1869,7 +1897,7 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
     </row>
-    <row r="46" spans="2:24" ht="30" customHeight="1">
+    <row r="46" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B46" s="6"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1894,7 +1922,7 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
-    <row r="47" spans="2:24" ht="30" customHeight="1">
+    <row r="47" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B47" s="6"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1919,7 +1947,7 @@
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
     </row>
-    <row r="48" spans="2:24" ht="30" customHeight="1">
+    <row r="48" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B48" s="6"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1944,7 +1972,7 @@
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
     </row>
-    <row r="49" spans="2:24" ht="30" customHeight="1">
+    <row r="49" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B49" s="6"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1969,7 +1997,7 @@
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
     </row>
-    <row r="50" spans="2:24" ht="30" customHeight="1">
+    <row r="50" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B50" s="6"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1994,7 +2022,7 @@
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
     </row>
-    <row r="51" spans="2:24" ht="30" customHeight="1">
+    <row r="51" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B51" s="6"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2019,7 +2047,7 @@
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
     </row>
-    <row r="52" spans="2:24" ht="30" customHeight="1">
+    <row r="52" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B52" s="6"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2044,7 +2072,7 @@
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
     </row>
-    <row r="53" spans="2:24" ht="30" customHeight="1">
+    <row r="53" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B53" s="6"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -2069,7 +2097,7 @@
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
     </row>
-    <row r="54" spans="2:24" ht="30" customHeight="1">
+    <row r="54" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B54" s="6"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2094,7 +2122,7 @@
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
     </row>
-    <row r="55" spans="2:24" ht="30" customHeight="1">
+    <row r="55" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B55" s="6"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2119,7 +2147,7 @@
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
     </row>
-    <row r="56" spans="2:24" ht="30" customHeight="1">
+    <row r="56" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B56" s="6"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2144,7 +2172,7 @@
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="2:24" ht="30" customHeight="1">
+    <row r="57" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B57" s="6"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2169,7 +2197,7 @@
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="2:24" ht="30" customHeight="1">
+    <row r="58" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B58" s="6"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2194,7 +2222,7 @@
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
     </row>
-    <row r="59" spans="2:24" ht="30" customHeight="1">
+    <row r="59" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B59" s="6"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2219,7 +2247,7 @@
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
     </row>
-    <row r="60" spans="2:24" ht="30" customHeight="1">
+    <row r="60" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B60" s="6"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2244,7 +2272,7 @@
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
     </row>
-    <row r="61" spans="2:24" ht="30" customHeight="1">
+    <row r="61" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B61" s="6"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2269,7 +2297,7 @@
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
     </row>
-    <row r="62" spans="2:24" ht="30" customHeight="1">
+    <row r="62" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B62" s="6"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2294,7 +2322,7 @@
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
     </row>
-    <row r="63" spans="2:24" ht="30" customHeight="1">
+    <row r="63" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B63" s="6"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -2319,7 +2347,7 @@
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
     </row>
-    <row r="64" spans="2:24" ht="30" customHeight="1">
+    <row r="64" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B64" s="6"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2344,7 +2372,7 @@
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
     </row>
-    <row r="65" spans="2:24" ht="30" customHeight="1">
+    <row r="65" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B65" s="6"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2369,7 +2397,7 @@
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
     </row>
-    <row r="66" spans="2:24" ht="30" customHeight="1">
+    <row r="66" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B66" s="6"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2394,7 +2422,7 @@
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="2:24" ht="30" customHeight="1">
+    <row r="67" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B67" s="6"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2419,7 +2447,7 @@
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="2:24" ht="30" customHeight="1">
+    <row r="68" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -2444,7 +2472,7 @@
       <c r="W68" s="7"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="2:24" ht="30" customHeight="1">
+    <row r="69" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -2469,7 +2497,7 @@
       <c r="W69" s="7"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="2:24" ht="30" customHeight="1">
+    <row r="70" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -2494,7 +2522,7 @@
       <c r="W70" s="7"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="2:24" ht="30" customHeight="1">
+    <row r="71" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -2519,7 +2547,7 @@
       <c r="W71" s="7"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="72" spans="2:24" ht="30" customHeight="1">
+    <row r="72" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B72" s="6"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -2544,7 +2572,7 @@
       <c r="W72" s="7"/>
       <c r="X72" s="3"/>
     </row>
-    <row r="73" spans="2:24" ht="30" customHeight="1">
+    <row r="73" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B73" s="6"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -2569,7 +2597,7 @@
       <c r="W73" s="7"/>
       <c r="X73" s="3"/>
     </row>
-    <row r="74" spans="2:24" ht="30" customHeight="1">
+    <row r="74" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B74" s="6"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -2594,7 +2622,7 @@
       <c r="W74" s="7"/>
       <c r="X74" s="3"/>
     </row>
-    <row r="75" spans="2:24" ht="30" customHeight="1">
+    <row r="75" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B75" s="6"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -2619,7 +2647,7 @@
       <c r="W75" s="7"/>
       <c r="X75" s="3"/>
     </row>
-    <row r="76" spans="2:24" ht="30" customHeight="1">
+    <row r="76" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B76" s="6"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -2644,7 +2672,7 @@
       <c r="W76" s="7"/>
       <c r="X76" s="3"/>
     </row>
-    <row r="77" spans="2:24" ht="30" customHeight="1">
+    <row r="77" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -2669,7 +2697,7 @@
       <c r="W77" s="7"/>
       <c r="X77" s="3"/>
     </row>
-    <row r="78" spans="2:24" ht="30" customHeight="1">
+    <row r="78" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B78" s="6"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -2694,7 +2722,7 @@
       <c r="W78" s="7"/>
       <c r="X78" s="3"/>
     </row>
-    <row r="79" spans="2:24" ht="30" customHeight="1">
+    <row r="79" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B79" s="6"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -2719,7 +2747,7 @@
       <c r="W79" s="7"/>
       <c r="X79" s="3"/>
     </row>
-    <row r="80" spans="2:24" ht="30" customHeight="1">
+    <row r="80" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B80" s="6"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -2744,7 +2772,7 @@
       <c r="W80" s="7"/>
       <c r="X80" s="3"/>
     </row>
-    <row r="81" spans="2:24" ht="30" customHeight="1">
+    <row r="81" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -2769,7 +2797,7 @@
       <c r="W81" s="7"/>
       <c r="X81" s="3"/>
     </row>
-    <row r="82" spans="2:24" ht="30" customHeight="1">
+    <row r="82" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -2794,7 +2822,7 @@
       <c r="W82" s="7"/>
       <c r="X82" s="3"/>
     </row>
-    <row r="83" spans="2:24" ht="30" customHeight="1">
+    <row r="83" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -2819,7 +2847,7 @@
       <c r="W83" s="7"/>
       <c r="X83" s="3"/>
     </row>
-    <row r="84" spans="2:24" ht="30" customHeight="1">
+    <row r="84" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B84" s="6"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -2844,7 +2872,7 @@
       <c r="W84" s="7"/>
       <c r="X84" s="3"/>
     </row>
-    <row r="85" spans="2:24" ht="30" customHeight="1">
+    <row r="85" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -2869,7 +2897,7 @@
       <c r="W85" s="7"/>
       <c r="X85" s="3"/>
     </row>
-    <row r="86" spans="2:24" ht="30" customHeight="1">
+    <row r="86" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B86" s="6"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -2894,7 +2922,7 @@
       <c r="W86" s="7"/>
       <c r="X86" s="3"/>
     </row>
-    <row r="87" spans="2:24" ht="30" customHeight="1">
+    <row r="87" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -2919,7 +2947,7 @@
       <c r="W87" s="7"/>
       <c r="X87" s="3"/>
     </row>
-    <row r="88" spans="2:24" ht="30" customHeight="1">
+    <row r="88" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -2944,7 +2972,7 @@
       <c r="W88" s="7"/>
       <c r="X88" s="3"/>
     </row>
-    <row r="89" spans="2:24" ht="30" customHeight="1">
+    <row r="89" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -2969,7 +2997,7 @@
       <c r="W89" s="7"/>
       <c r="X89" s="3"/>
     </row>
-    <row r="90" spans="2:24" ht="30" customHeight="1">
+    <row r="90" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -2994,7 +3022,7 @@
       <c r="W90" s="7"/>
       <c r="X90" s="3"/>
     </row>
-    <row r="91" spans="2:24" ht="30" customHeight="1">
+    <row r="91" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -3019,7 +3047,7 @@
       <c r="W91" s="7"/>
       <c r="X91" s="3"/>
     </row>
-    <row r="92" spans="2:24" ht="30" customHeight="1">
+    <row r="92" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B92" s="6"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -3044,7 +3072,7 @@
       <c r="W92" s="7"/>
       <c r="X92" s="3"/>
     </row>
-    <row r="93" spans="2:24" ht="30" customHeight="1">
+    <row r="93" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -3069,7 +3097,7 @@
       <c r="W93" s="7"/>
       <c r="X93" s="3"/>
     </row>
-    <row r="94" spans="2:24" ht="30" customHeight="1">
+    <row r="94" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B94" s="6"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -3094,7 +3122,7 @@
       <c r="W94" s="7"/>
       <c r="X94" s="3"/>
     </row>
-    <row r="95" spans="2:24" ht="30" customHeight="1">
+    <row r="95" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B95" s="6"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -3119,7 +3147,7 @@
       <c r="W95" s="7"/>
       <c r="X95" s="3"/>
     </row>
-    <row r="96" spans="2:24" ht="30" customHeight="1">
+    <row r="96" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -3144,7 +3172,7 @@
       <c r="W96" s="7"/>
       <c r="X96" s="3"/>
     </row>
-    <row r="97" spans="2:24" ht="30" customHeight="1">
+    <row r="97" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B97" s="6"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -3169,7 +3197,7 @@
       <c r="W97" s="7"/>
       <c r="X97" s="3"/>
     </row>
-    <row r="98" spans="2:24" ht="30" customHeight="1">
+    <row r="98" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B98" s="6"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -3194,7 +3222,7 @@
       <c r="W98" s="7"/>
       <c r="X98" s="3"/>
     </row>
-    <row r="99" spans="2:24" ht="30" customHeight="1">
+    <row r="99" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B99" s="6"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -3219,7 +3247,7 @@
       <c r="W99" s="7"/>
       <c r="X99" s="3"/>
     </row>
-    <row r="100" spans="2:24" ht="30" customHeight="1">
+    <row r="100" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B100" s="6"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -3244,7 +3272,7 @@
       <c r="W100" s="7"/>
       <c r="X100" s="3"/>
     </row>
-    <row r="101" spans="2:24" ht="30" customHeight="1">
+    <row r="101" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B101" s="6"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -3269,7 +3297,7 @@
       <c r="W101" s="7"/>
       <c r="X101" s="3"/>
     </row>
-    <row r="102" spans="2:24" ht="30" customHeight="1">
+    <row r="102" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B102" s="6"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -3294,7 +3322,7 @@
       <c r="W102" s="7"/>
       <c r="X102" s="3"/>
     </row>
-    <row r="103" spans="2:24" ht="30" customHeight="1">
+    <row r="103" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B103" s="6"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -3319,7 +3347,7 @@
       <c r="W103" s="7"/>
       <c r="X103" s="3"/>
     </row>
-    <row r="104" spans="2:24" ht="30" customHeight="1">
+    <row r="104" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B104" s="6"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -3344,7 +3372,7 @@
       <c r="W104" s="7"/>
       <c r="X104" s="3"/>
     </row>
-    <row r="105" spans="2:24" ht="30" customHeight="1">
+    <row r="105" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B105" s="6"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -3369,7 +3397,7 @@
       <c r="W105" s="7"/>
       <c r="X105" s="3"/>
     </row>
-    <row r="106" spans="2:24" ht="30" customHeight="1">
+    <row r="106" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B106" s="6"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -3394,7 +3422,7 @@
       <c r="W106" s="7"/>
       <c r="X106" s="3"/>
     </row>
-    <row r="107" spans="2:24" ht="30" customHeight="1">
+    <row r="107" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B107" s="6"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -3419,7 +3447,7 @@
       <c r="W107" s="7"/>
       <c r="X107" s="3"/>
     </row>
-    <row r="108" spans="2:24" ht="30" customHeight="1">
+    <row r="108" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B108" s="6"/>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -3444,7 +3472,7 @@
       <c r="W108" s="7"/>
       <c r="X108" s="3"/>
     </row>
-    <row r="109" spans="2:24" ht="30" customHeight="1">
+    <row r="109" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B109" s="6"/>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -3469,7 +3497,7 @@
       <c r="W109" s="7"/>
       <c r="X109" s="3"/>
     </row>
-    <row r="110" spans="2:24" ht="30" customHeight="1">
+    <row r="110" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B110" s="6"/>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -3494,7 +3522,7 @@
       <c r="W110" s="7"/>
       <c r="X110" s="3"/>
     </row>
-    <row r="111" spans="2:24" ht="30" customHeight="1">
+    <row r="111" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B111" s="6"/>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -3519,7 +3547,7 @@
       <c r="W111" s="7"/>
       <c r="X111" s="3"/>
     </row>
-    <row r="112" spans="2:24" ht="30" customHeight="1">
+    <row r="112" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B112" s="6"/>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
@@ -3544,7 +3572,7 @@
       <c r="W112" s="7"/>
       <c r="X112" s="3"/>
     </row>
-    <row r="113" spans="2:24" ht="30" customHeight="1">
+    <row r="113" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B113" s="6"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -3569,7 +3597,7 @@
       <c r="W113" s="7"/>
       <c r="X113" s="3"/>
     </row>
-    <row r="114" spans="2:24" ht="30" customHeight="1">
+    <row r="114" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B114" s="6"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
@@ -3594,7 +3622,7 @@
       <c r="W114" s="7"/>
       <c r="X114" s="3"/>
     </row>
-    <row r="115" spans="2:24" ht="30" customHeight="1">
+    <row r="115" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B115" s="6"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -3619,7 +3647,7 @@
       <c r="W115" s="7"/>
       <c r="X115" s="3"/>
     </row>
-    <row r="116" spans="2:24" ht="30" customHeight="1">
+    <row r="116" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B116" s="6"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
@@ -3644,7 +3672,7 @@
       <c r="W116" s="7"/>
       <c r="X116" s="3"/>
     </row>
-    <row r="117" spans="2:24" ht="30" customHeight="1">
+    <row r="117" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B117" s="6"/>
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
@@ -3669,7 +3697,7 @@
       <c r="W117" s="7"/>
       <c r="X117" s="3"/>
     </row>
-    <row r="118" spans="2:24" ht="30" customHeight="1">
+    <row r="118" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B118" s="6"/>
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
@@ -3694,7 +3722,7 @@
       <c r="W118" s="7"/>
       <c r="X118" s="3"/>
     </row>
-    <row r="119" spans="2:24" ht="30" customHeight="1">
+    <row r="119" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B119" s="6"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
@@ -3719,7 +3747,7 @@
       <c r="W119" s="7"/>
       <c r="X119" s="3"/>
     </row>
-    <row r="120" spans="2:24" ht="30" customHeight="1">
+    <row r="120" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B120" s="6"/>
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
@@ -3744,7 +3772,7 @@
       <c r="W120" s="7"/>
       <c r="X120" s="3"/>
     </row>
-    <row r="121" spans="2:24" ht="30" customHeight="1">
+    <row r="121" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B121" s="6"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
@@ -3769,7 +3797,7 @@
       <c r="W121" s="7"/>
       <c r="X121" s="3"/>
     </row>
-    <row r="122" spans="2:24" ht="30" customHeight="1">
+    <row r="122" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B122" s="6"/>
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
@@ -3794,7 +3822,7 @@
       <c r="W122" s="7"/>
       <c r="X122" s="3"/>
     </row>
-    <row r="123" spans="2:24" ht="30" customHeight="1">
+    <row r="123" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B123" s="6"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
@@ -3819,7 +3847,7 @@
       <c r="W123" s="7"/>
       <c r="X123" s="3"/>
     </row>
-    <row r="124" spans="2:24" ht="30" customHeight="1">
+    <row r="124" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B124" s="6"/>
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
@@ -3844,7 +3872,7 @@
       <c r="W124" s="7"/>
       <c r="X124" s="3"/>
     </row>
-    <row r="125" spans="2:24" ht="30" customHeight="1">
+    <row r="125" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B125" s="6"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
@@ -3869,7 +3897,7 @@
       <c r="W125" s="7"/>
       <c r="X125" s="3"/>
     </row>
-    <row r="126" spans="2:24" ht="30" customHeight="1">
+    <row r="126" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B126" s="6"/>
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
@@ -3894,7 +3922,7 @@
       <c r="W126" s="7"/>
       <c r="X126" s="3"/>
     </row>
-    <row r="127" spans="2:24" ht="30" customHeight="1">
+    <row r="127" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B127" s="6"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
@@ -3919,7 +3947,7 @@
       <c r="W127" s="7"/>
       <c r="X127" s="3"/>
     </row>
-    <row r="128" spans="2:24" ht="30" customHeight="1">
+    <row r="128" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B128" s="6"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
@@ -3944,7 +3972,7 @@
       <c r="W128" s="7"/>
       <c r="X128" s="3"/>
     </row>
-    <row r="129" spans="2:24" ht="30" customHeight="1">
+    <row r="129" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B129" s="6"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
@@ -3969,7 +3997,7 @@
       <c r="W129" s="7"/>
       <c r="X129" s="3"/>
     </row>
-    <row r="130" spans="2:24" ht="30" customHeight="1">
+    <row r="130" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B130" s="6"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
@@ -3994,7 +4022,7 @@
       <c r="W130" s="7"/>
       <c r="X130" s="3"/>
     </row>
-    <row r="131" spans="2:24" ht="30" customHeight="1">
+    <row r="131" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B131" s="6"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
@@ -4019,7 +4047,7 @@
       <c r="W131" s="7"/>
       <c r="X131" s="3"/>
     </row>
-    <row r="132" spans="2:24" ht="30" customHeight="1">
+    <row r="132" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B132" s="6"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
@@ -4044,7 +4072,7 @@
       <c r="W132" s="7"/>
       <c r="X132" s="3"/>
     </row>
-    <row r="133" spans="2:24" ht="30" customHeight="1">
+    <row r="133" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B133" s="6"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
@@ -4069,7 +4097,7 @@
       <c r="W133" s="7"/>
       <c r="X133" s="3"/>
     </row>
-    <row r="134" spans="2:24" ht="30" customHeight="1">
+    <row r="134" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B134" s="6"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
@@ -4094,7 +4122,7 @@
       <c r="W134" s="7"/>
       <c r="X134" s="3"/>
     </row>
-    <row r="135" spans="2:24" ht="30" customHeight="1">
+    <row r="135" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B135" s="6"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
@@ -4119,7 +4147,7 @@
       <c r="W135" s="7"/>
       <c r="X135" s="3"/>
     </row>
-    <row r="136" spans="2:24" ht="30" customHeight="1">
+    <row r="136" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B136" s="6"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
@@ -4144,7 +4172,7 @@
       <c r="W136" s="7"/>
       <c r="X136" s="3"/>
     </row>
-    <row r="137" spans="2:24" ht="30" customHeight="1">
+    <row r="137" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B137" s="6"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
@@ -4169,7 +4197,7 @@
       <c r="W137" s="7"/>
       <c r="X137" s="3"/>
     </row>
-    <row r="138" spans="2:24" ht="30" customHeight="1">
+    <row r="138" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B138" s="6"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
@@ -4194,7 +4222,7 @@
       <c r="W138" s="7"/>
       <c r="X138" s="3"/>
     </row>
-    <row r="139" spans="2:24" ht="30" customHeight="1">
+    <row r="139" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B139" s="6"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
@@ -4219,7 +4247,7 @@
       <c r="W139" s="7"/>
       <c r="X139" s="3"/>
     </row>
-    <row r="140" spans="2:24" ht="30" customHeight="1">
+    <row r="140" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B140" s="6"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
@@ -4244,7 +4272,7 @@
       <c r="W140" s="7"/>
       <c r="X140" s="3"/>
     </row>
-    <row r="141" spans="2:24" ht="30" customHeight="1">
+    <row r="141" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B141" s="6"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
@@ -4269,7 +4297,7 @@
       <c r="W141" s="7"/>
       <c r="X141" s="3"/>
     </row>
-    <row r="142" spans="2:24" ht="30" customHeight="1">
+    <row r="142" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B142" s="6"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
@@ -4294,106 +4322,95 @@
       <c r="W142" s="7"/>
       <c r="X142" s="3"/>
     </row>
-    <row r="143" spans="2:24" ht="30" customHeight="1">
+    <row r="143" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B143" s="8"/>
       <c r="X143" s="9"/>
     </row>
-    <row r="144" spans="2:24" ht="30" customHeight="1">
+    <row r="144" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B144" s="8"/>
       <c r="X144" s="9"/>
     </row>
-    <row r="145" spans="2:24" ht="30" customHeight="1">
+    <row r="145" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B145" s="8"/>
       <c r="X145" s="9"/>
     </row>
-    <row r="146" spans="2:24" ht="30" customHeight="1">
+    <row r="146" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B146" s="8"/>
       <c r="X146" s="9"/>
     </row>
-    <row r="147" spans="2:24" ht="30" customHeight="1">
+    <row r="147" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B147" s="8"/>
       <c r="X147" s="9"/>
     </row>
-    <row r="148" spans="2:24" ht="30" customHeight="1">
+    <row r="148" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B148" s="8"/>
       <c r="X148" s="9"/>
     </row>
-    <row r="149" spans="2:24" ht="30" customHeight="1">
+    <row r="149" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B149" s="8"/>
       <c r="X149" s="9"/>
     </row>
-    <row r="150" spans="2:24" ht="30" customHeight="1">
+    <row r="150" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B150" s="8"/>
       <c r="X150" s="9"/>
     </row>
-    <row r="151" spans="2:24" ht="30" customHeight="1">
+    <row r="151" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B151" s="8"/>
       <c r="X151" s="9"/>
     </row>
-    <row r="152" spans="2:24" ht="30" customHeight="1">
+    <row r="152" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B152" s="8"/>
       <c r="X152" s="9"/>
     </row>
-    <row r="153" spans="2:24" ht="30" customHeight="1">
+    <row r="153" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B153" s="8"/>
       <c r="X153" s="9"/>
     </row>
-    <row r="154" spans="2:24" ht="30" customHeight="1">
+    <row r="154" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B154" s="8"/>
       <c r="X154" s="9"/>
     </row>
-    <row r="155" spans="2:24" ht="30" customHeight="1">
+    <row r="155" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B155" s="8"/>
       <c r="X155" s="9"/>
     </row>
-    <row r="156" spans="2:24" ht="30" customHeight="1">
+    <row r="156" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B156" s="8"/>
       <c r="X156" s="9"/>
     </row>
-    <row r="157" spans="2:24" ht="30" customHeight="1">
+    <row r="157" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B157" s="8"/>
       <c r="X157" s="9"/>
     </row>
-    <row r="158" spans="2:24" ht="30" customHeight="1">
+    <row r="158" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B158" s="8"/>
     </row>
-    <row r="159" spans="2:24" ht="30" customHeight="1">
+    <row r="159" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B159" s="8"/>
     </row>
-    <row r="160" spans="2:24" ht="30" customHeight="1">
+    <row r="160" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B160" s="8"/>
     </row>
-    <row r="161" spans="2:2" ht="30" customHeight="1">
+    <row r="161" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B161" s="8"/>
     </row>
-    <row r="162" spans="2:2" ht="30" customHeight="1">
+    <row r="162" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B162" s="8"/>
     </row>
-    <row r="163" spans="2:2" ht="30" customHeight="1">
+    <row r="163" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B163" s="8"/>
     </row>
-    <row r="164" spans="2:2" ht="30" customHeight="1">
+    <row r="164" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B164" s="8"/>
     </row>
-    <row r="165" spans="2:2" ht="30" customHeight="1">
+    <row r="165" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B165" s="8"/>
     </row>
-    <row r="166" spans="2:2" ht="30" customHeight="1">
+    <row r="166" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B166" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
@@ -4406,6 +4423,17 @@
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ตรวจ Burndown Velocity Sprint 8
</commit_message>
<xml_diff>
--- a/ตรวจงาน/รายการตรวจสอบเอกสารอื่น ๆ.xlsx
+++ b/ตรวจงาน/รายการตรวจสอบเอกสารอื่น ๆ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\team4\ตรวจงาน\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8743BE70-F858-4D20-83CF-06191B77747F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455F1794-2909-43D9-958E-C85B5562C88E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C108298C-C5B1-4B19-85F2-2856099ECD84}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>คำผิด</t>
   </si>
@@ -155,6 +155,12 @@
   <si>
     <t>1.8.1</t>
   </si>
+  <si>
+    <t>Burndown Velocity Sprint 1-8</t>
+  </si>
+  <si>
+    <t>1.9.1</t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -292,7 +298,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -303,12 +318,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,7 +636,7 @@
   <dimension ref="B2:X166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.7"/>
@@ -640,100 +649,100 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="50.4" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="Q2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:24" ht="51.75" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
     </row>
     <row r="4" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B4" s="2" t="s">
@@ -1048,10 +1057,18 @@
       </c>
     </row>
     <row r="12" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B12" s="6"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44429</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1070,7 +1087,9 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
+      <c r="X12" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:24" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B13" s="6"/>
@@ -4411,6 +4430,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
@@ -4423,17 +4453,6 @@
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>